<commit_message>
update cost-based reference data to MIP model results
</commit_message>
<xml_diff>
--- a/endoresults/results.xlsx
+++ b/endoresults/results.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/canli/euler/work/GETP/endoresults/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCA7D6C0-933F-7542-BEDC-54E5CC29C10D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8CEA024-616C-B643-A50E-481EA0FD048A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="19400" activeTab="1" xr2:uid="{AEA648F7-838F-4A48-9949-F171A1DAE8D2}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="28">
   <si>
     <t>LB</t>
   </si>
@@ -76,16 +76,68 @@
   </si>
   <si>
     <t>instance</t>
+  </si>
+  <si>
+    <t>high var means DIC =[0.1, 1.0, 1.9] of nomial value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">low var:DIC=[0.3, 1.0, 1.3] </t>
+  </si>
+  <si>
+    <t>5 years, 5 days low ng price</t>
+  </si>
+  <si>
+    <t xml:space="preserve">more tests with medim carbon tax </t>
+  </si>
+  <si>
+    <t>coal-new-igcc</t>
+  </si>
+  <si>
+    <t>coal-igcc-css-new</t>
+  </si>
+  <si>
+    <t>DIC= [0.2 1.0, 1.3], high ng</t>
+  </si>
+  <si>
+    <t>DIC= [0.1 1.0, 1.3], high ng</t>
+  </si>
+  <si>
+    <t>solution description</t>
+  </si>
+  <si>
+    <t>DIC= [0.2 1.0, 1.3], high ng * 1.5</t>
+  </si>
+  <si>
+    <t>DIC= [0.5 1.0, 1.3], high ng * 1.5</t>
+  </si>
+  <si>
+    <t>1 coal plant installed at t=1. Continue installation for low price scenario</t>
+  </si>
+  <si>
+    <t>time limit: 43200 secs</t>
+  </si>
+  <si>
+    <t>no coal plant installed in all scenarios</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="0.0%"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -131,7 +183,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -170,6 +222,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -178,12 +239,6 @@
   </cellStyles>
   <dxfs count="22">
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="3" formatCode="#,##0"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -209,13 +264,6 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
     </dxf>
     <dxf>
       <border outline="0">
@@ -231,41 +279,41 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <border outline="0">
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
       </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <border outline="0">
@@ -276,6 +324,19 @@
           <color indexed="64"/>
         </bottom>
       </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -291,34 +352,34 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{729DAF8D-A289-5043-B673-D6184CA4041D}" name="Table1" displayName="Table1" ref="I2:O6" totalsRowShown="0" headerRowDxfId="11" dataDxfId="12" headerRowBorderDxfId="20" tableBorderDxfId="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{729DAF8D-A289-5043-B673-D6184CA4041D}" name="Table1" displayName="Table1" ref="I2:O6" totalsRowShown="0" headerRowDxfId="21" dataDxfId="19" headerRowBorderDxfId="20" tableBorderDxfId="18">
   <autoFilter ref="I2:O6" xr:uid="{CEA701A5-7AD5-734F-860B-11F405B82502}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{93C1109B-B9AF-7B4D-A5FF-0014D9D5B1DB}" name="Column1" dataDxfId="19"/>
-    <tableColumn id="2" xr3:uid="{66876046-CD3C-554A-A9BE-D2BC3485285C}" name="LB" dataDxfId="18"/>
-    <tableColumn id="3" xr3:uid="{6C46065A-734A-E346-91C3-5C971FDA7F75}" name="UB" dataDxfId="17"/>
-    <tableColumn id="4" xr3:uid="{A8228276-C6CE-BC4B-9871-1F13E2BF7F59}" name="Gap" dataDxfId="16">
+    <tableColumn id="1" xr3:uid="{93C1109B-B9AF-7B4D-A5FF-0014D9D5B1DB}" name="Column1" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{66876046-CD3C-554A-A9BE-D2BC3485285C}" name="LB" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{6C46065A-734A-E346-91C3-5C971FDA7F75}" name="UB" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{A8228276-C6CE-BC4B-9871-1F13E2BF7F59}" name="Gap" dataDxfId="14">
       <calculatedColumnFormula>(K3-J3)/K3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{2EAACD3A-2B85-754D-8BCF-E43F018DA9BC}" name="LP time" dataDxfId="15"/>
-    <tableColumn id="6" xr3:uid="{65A9F7F8-6C55-9348-8419-EB14F8C3F540}" name="Heuristic time" dataDxfId="14"/>
-    <tableColumn id="7" xr3:uid="{72BEB32A-B80D-EC44-A0F4-E949F7740C33}" name="Wall time" dataDxfId="13"/>
+    <tableColumn id="5" xr3:uid="{2EAACD3A-2B85-754D-8BCF-E43F018DA9BC}" name="LP time" dataDxfId="13"/>
+    <tableColumn id="6" xr3:uid="{65A9F7F8-6C55-9348-8419-EB14F8C3F540}" name="Heuristic time" dataDxfId="12"/>
+    <tableColumn id="7" xr3:uid="{72BEB32A-B80D-EC44-A0F4-E949F7740C33}" name="Wall time" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{81E8BE08-1A91-6F41-B41E-5183DE645003}" name="Table2" displayName="Table2" ref="J2:P6" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1" headerRowBorderDxfId="9" tableBorderDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{81E8BE08-1A91-6F41-B41E-5183DE645003}" name="Table2" displayName="Table2" ref="J2:P6" totalsRowShown="0" headerRowDxfId="10" dataDxfId="8" headerRowBorderDxfId="9" tableBorderDxfId="7">
   <autoFilter ref="J2:P6" xr:uid="{903A0441-986F-7846-B62E-2EFD47E5FA34}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{FCDF9D90-CB2B-314F-9A07-EC3841EBFA59}" name="instance" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{DFDD54D1-F489-4F4B-A7B0-31E3D19EF7D0}" name="LB" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{0FD91812-3182-EB46-AE77-7CA4FBF9820E}" name="UB" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{44660A07-6B3C-F94E-A952-ABE7033425A5}" name="Gap" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{16B90C05-02E0-6C47-B4A1-F3A58DA024E7}" name="Benders time" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{19A27586-950B-DF4D-8494-D8A1BD0B9216}" name="Heuristic time" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{BAD4D4C1-088D-1743-8124-FCC314F2872D}" name="Wall time" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{FCDF9D90-CB2B-314F-9A07-EC3841EBFA59}" name="instance" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{DFDD54D1-F489-4F4B-A7B0-31E3D19EF7D0}" name="LB" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{0FD91812-3182-EB46-AE77-7CA4FBF9820E}" name="UB" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{44660A07-6B3C-F94E-A952-ABE7033425A5}" name="Gap" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{16B90C05-02E0-6C47-B4A1-F3A58DA024E7}" name="Benders time" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{19A27586-950B-DF4D-8494-D8A1BD0B9216}" name="Heuristic time" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{BAD4D4C1-088D-1743-8124-FCC314F2872D}" name="Wall time" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -881,17 +942,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF1C1643-1B25-7B40-B346-02E652E25DE0}">
-  <dimension ref="A1:P6"/>
+  <dimension ref="A1:P15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="61" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="18.83203125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="13.83203125" customWidth="1"/>
     <col min="15" max="15" width="14.5" customWidth="1"/>
@@ -900,7 +962,16 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
@@ -1105,6 +1176,155 @@
       <c r="O6" s="13"/>
       <c r="P6" s="13"/>
     </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H11" s="14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="2">
+        <f>77997.32707/1000</f>
+        <v>77.997327069999997</v>
+      </c>
+      <c r="C12" s="2">
+        <f>78949.46069/1000</f>
+        <v>78.949460690000009</v>
+      </c>
+      <c r="D12" s="15">
+        <f>(C12-B12)/C12</f>
+        <v>1.2060039570613716E-2</v>
+      </c>
+      <c r="E12" s="4">
+        <v>43200</v>
+      </c>
+      <c r="F12" s="4">
+        <v>273</v>
+      </c>
+      <c r="G12" s="4">
+        <v>44970</v>
+      </c>
+      <c r="H12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="2">
+        <f>76629/1000</f>
+        <v>76.629000000000005</v>
+      </c>
+      <c r="C13" s="2">
+        <v>77.599999999999994</v>
+      </c>
+      <c r="D13" s="15">
+        <f t="shared" ref="D13:D15" si="2">(C13-B13)/C13</f>
+        <v>1.2512886597938009E-2</v>
+      </c>
+      <c r="E13" s="4">
+        <v>43200</v>
+      </c>
+      <c r="F13" s="4">
+        <v>291</v>
+      </c>
+      <c r="G13" s="4">
+        <v>45036</v>
+      </c>
+      <c r="H13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="2">
+        <f>86701/1000</f>
+        <v>86.700999999999993</v>
+      </c>
+      <c r="C14" s="2">
+        <v>87.334999999999994</v>
+      </c>
+      <c r="D14" s="15">
+        <f t="shared" si="2"/>
+        <v>7.2594034464991174E-3</v>
+      </c>
+      <c r="E14" s="4">
+        <v>43200</v>
+      </c>
+      <c r="F14" s="4">
+        <v>282</v>
+      </c>
+      <c r="G14" s="4">
+        <v>45047</v>
+      </c>
+      <c r="H14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A15" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="2">
+        <v>90.274000000000001</v>
+      </c>
+      <c r="C15" s="2">
+        <v>90.841999999999999</v>
+      </c>
+      <c r="D15" s="15">
+        <f t="shared" si="2"/>
+        <v>6.2526144294489097E-3</v>
+      </c>
+      <c r="E15" s="4">
+        <v>43200</v>
+      </c>
+      <c r="F15" s="4">
+        <v>89</v>
+      </c>
+      <c r="G15" s="4">
+        <v>44763</v>
+      </c>
+      <c r="H15" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>